<commit_message>
added ster & nouse by education and age at first birth
</commit_message>
<xml_diff>
--- a/vartx_charts.xlsx
+++ b/vartx_charts.xlsx
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24525" windowHeight="12330" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="nouse" sheetId="1" r:id="rId1"/>
     <sheet name="ster" sheetId="2" r:id="rId2"/>
     <sheet name="allrepro_contage" sheetId="3" r:id="rId3"/>
     <sheet name="allrepro_catage" sheetId="4" r:id="rId4"/>
+    <sheet name="nouse_edu" sheetId="5" r:id="rId5"/>
+    <sheet name="ster_edu" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="74">
   <si>
     <t>15 YEARS</t>
   </si>
@@ -217,6 +220,39 @@
   <si>
     <t>40-44</t>
   </si>
+  <si>
+    <t>no hs degree</t>
+  </si>
+  <si>
+    <t>hs degree or ged</t>
+  </si>
+  <si>
+    <t>some college no degree</t>
+  </si>
+  <si>
+    <t>associate's</t>
+  </si>
+  <si>
+    <t>bachelor's</t>
+  </si>
+  <si>
+    <t>graduate or professional degree</t>
+  </si>
+  <si>
+    <t>using reversible contraception</t>
+  </si>
+  <si>
+    <t>UNDER 20 YEARS</t>
+  </si>
+  <si>
+    <t>20-24 YEARS</t>
+  </si>
+  <si>
+    <t>25-29 YEARS</t>
+  </si>
+  <si>
+    <t>30-44 YEARS</t>
+  </si>
 </sst>
 </file>
 
@@ -285,6 +321,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Not Using Contraception</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -348,103 +409,100 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>nouse!$B$3:$AG$3</c:f>
+              <c:f>nouse!$B$3:$AF$3</c:f>
               <c:strCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>15 YEARS</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16 YEARS</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17 YEARS</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18 YEARS</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19 YEARS</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20 YEARS</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21 YEARS</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22 YEARS</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23 YEARS</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24 YEARS</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25 YEARS</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26 YEARS</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27 YEARS</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28 YEARS</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29 YEARS</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>30 YEARS</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>31 YEARS</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32 YEARS</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>33 YEARS</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34 YEARS</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>35 YEARS</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>36 YEARS</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>37 YEARS</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>38 YEARS</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>39 YEARS</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>40 YEARS</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41 YEARS</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42 YEARS</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43 YEARS</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>44 YEARS</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>NOT ASCERTAINED</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>Total</c:v>
                 </c:pt>
               </c:strCache>
@@ -452,10 +510,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>nouse!$B$5:$AG$5</c:f>
+              <c:f>nouse!$B$5:$AF$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>14.29</c:v>
                 </c:pt>
@@ -545,9 +603,6 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>9.7200000000000006</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -578,6 +633,62 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Age</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -643,6 +754,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>%</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5727,6 +5894,956 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nouse_edu!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>not using anything</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>nouse_edu!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>no hs degree</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>hs degree or ged</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>some college no degree</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>associate's</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>bachelor's</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>graduate or professional degree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>nouse_edu!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>13.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A0E8-4C03-B045-34DD440371C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="10563295"/>
+        <c:axId val="160352879"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="10563295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="160352879"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="160352879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10563295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ster_edu!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sterilized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ster_edu!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>no hs degree</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>hs degree or ged</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>some college no degree</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>associate's</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>bachelor's</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>graduate or professional degree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ster_edu!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>33.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.46</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E10-4302-8DD3-3EA8B64B7069}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="149858975"/>
+        <c:axId val="149864383"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="149858975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="149864383"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="149864383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="149858975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>not using anything</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>UNDER 20 YEARS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20-24 YEARS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25-29 YEARS</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30-44 YEARS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1245-447F-AA92-A1F273A63CF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="152881839"/>
+        <c:axId val="152884335"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="152881839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="152884335"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="152884335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="152881839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5887,6 +7004,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -7871,6 +9108,1515 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -8021,6 +10767,111 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>38</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8306,113 +11157,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AG6"/>
+  <dimension ref="A3:AF6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" activeCellId="1" sqref="A3:XFD3 A5:XFD5"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="C3" sqref="B3:AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q3" t="s">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>15</v>
       </c>
-      <c r="R3" t="s">
+      <c r="C3">
         <v>16</v>
       </c>
-      <c r="S3" t="s">
+      <c r="D3">
         <v>17</v>
       </c>
-      <c r="T3" t="s">
+      <c r="E3">
         <v>18</v>
       </c>
-      <c r="U3" t="s">
+      <c r="F3">
         <v>19</v>
       </c>
-      <c r="V3" t="s">
+      <c r="G3">
         <v>20</v>
       </c>
-      <c r="W3" t="s">
+      <c r="H3">
         <v>21</v>
       </c>
-      <c r="X3" t="s">
+      <c r="I3">
         <v>22</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="J3">
         <v>23</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="K3">
         <v>24</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="L3">
         <v>25</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="M3">
         <v>26</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="N3">
         <v>27</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="O3">
         <v>28</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="P3">
         <v>29</v>
       </c>
+      <c r="Q3">
+        <v>30</v>
+      </c>
+      <c r="R3">
+        <v>31</v>
+      </c>
+      <c r="S3">
+        <v>32</v>
+      </c>
+      <c r="T3">
+        <v>33</v>
+      </c>
+      <c r="U3">
+        <v>34</v>
+      </c>
+      <c r="V3">
+        <v>35</v>
+      </c>
+      <c r="W3">
+        <v>36</v>
+      </c>
+      <c r="X3">
+        <v>37</v>
+      </c>
+      <c r="Y3">
+        <v>38</v>
+      </c>
+      <c r="Z3">
+        <v>39</v>
+      </c>
+      <c r="AA3">
+        <v>40</v>
+      </c>
+      <c r="AB3">
+        <v>41</v>
+      </c>
+      <c r="AC3">
+        <v>42</v>
+      </c>
+      <c r="AD3">
+        <v>43</v>
+      </c>
+      <c r="AE3">
+        <v>44</v>
+      </c>
       <c r="AF3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -8506,11 +11354,8 @@
       <c r="AE4">
         <v>90.28</v>
       </c>
-      <c r="AF4">
-        <v>100</v>
-      </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -8604,11 +11449,8 @@
       <c r="AE5">
         <v>9.7200000000000006</v>
       </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -8703,9 +11545,6 @@
         <v>216</v>
       </c>
       <c r="AF6">
-        <v>1</v>
-      </c>
-      <c r="AG6">
         <v>7505</v>
       </c>
     </row>
@@ -10721,7 +13560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:N10"/>
     </sheetView>
   </sheetViews>
@@ -10801,55 +13640,55 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
-        <f>CONCATENATE(B1," ",B2," ",B3)</f>
+        <f t="shared" ref="B4:N4" si="0">CONCATENATE(B1," ",B2," ",B3)</f>
         <v xml:space="preserve">sterilized  </v>
       </c>
       <c r="C4" t="str">
-        <f>CONCATENATE(C1," ",C2," ",C3)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">IUD, implant  </v>
       </c>
       <c r="D4" t="str">
-        <f>CONCATENATE(D1," ",D2," ",D3)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">injection, pill, patch, ring </v>
       </c>
       <c r="E4" t="str">
-        <f>CONCATENATE(E1," ",E2," ",E3)</f>
+        <f t="shared" si="0"/>
         <v>condom, diaphragm, sponge, foam, insert, jelly</v>
       </c>
       <c r="F4" t="str">
-        <f>CONCATENATE(F1," ",F2," ",F3)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">periodic abstinence  </v>
       </c>
       <c r="G4" t="str">
-        <f>CONCATENATE(G1," ",G2," ",G3)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">withdrawal  </v>
       </c>
       <c r="H4" t="str">
-        <f>CONCATENATE(H1," ",H2," ",H3)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">not using contraception  </v>
       </c>
       <c r="I4" t="str">
-        <f>CONCATENATE(I1," ",I2," ",I3)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">pregnant  </v>
       </c>
       <c r="J4" t="str">
-        <f>CONCATENATE(J1," ",J2," ",J3)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">seeking pregnancy  </v>
       </c>
       <c r="K4" t="str">
-        <f>CONCATENATE(K1," ",K2," ",K3)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">&lt; 2 months postpartum  </v>
       </c>
       <c r="L4" t="str">
-        <f>CONCATENATE(L1," ",L2," ",L3)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">noncontraceptive sterile </v>
       </c>
       <c r="M4" t="str">
-        <f>CONCATENATE(M1," ",M2," ",M3)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">never had intercourse since first period </v>
       </c>
       <c r="N4" t="str">
-        <f>CONCATENATE(N1," ",N2," ",N3)</f>
+        <f t="shared" si="0"/>
         <v>no intercourse in 3 months b4 interview</v>
       </c>
     </row>
@@ -11115,6 +13954,292 @@
       </c>
       <c r="N10">
         <v>10.199999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" activeCellId="1" sqref="A1:A7 C1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2">
+        <v>86.58</v>
+      </c>
+      <c r="C2">
+        <v>13.42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>90.68</v>
+      </c>
+      <c r="C3">
+        <v>9.32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>90.54</v>
+      </c>
+      <c r="C4">
+        <v>9.4600000000000009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>89.16</v>
+      </c>
+      <c r="C5">
+        <v>10.84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6">
+        <v>91.26</v>
+      </c>
+      <c r="C6">
+        <v>8.74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7">
+        <v>91.33</v>
+      </c>
+      <c r="C7">
+        <v>8.67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2">
+        <v>33.89</v>
+      </c>
+      <c r="C2">
+        <v>55.63</v>
+      </c>
+      <c r="D2">
+        <v>10.48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>30.37</v>
+      </c>
+      <c r="C3">
+        <v>62.73</v>
+      </c>
+      <c r="D3">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>23.46</v>
+      </c>
+      <c r="C4">
+        <v>69.44</v>
+      </c>
+      <c r="D4">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>26.24</v>
+      </c>
+      <c r="C5">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="D5">
+        <v>8.36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6">
+        <v>15.68</v>
+      </c>
+      <c r="C6">
+        <v>78.05</v>
+      </c>
+      <c r="D6">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7">
+        <v>18.93</v>
+      </c>
+      <c r="C7">
+        <v>74.61</v>
+      </c>
+      <c r="D7">
+        <v>6.45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" activeCellId="1" sqref="A1:A5 C1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2">
+        <v>92.65</v>
+      </c>
+      <c r="C2">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3">
+        <v>90.39</v>
+      </c>
+      <c r="C3">
+        <v>9.61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4">
+        <v>91.73</v>
+      </c>
+      <c r="C4">
+        <v>8.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5">
+        <v>87.9</v>
+      </c>
+      <c r="C5">
+        <v>12.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>